<commit_message>
updated charts - removed p-values
</commit_message>
<xml_diff>
--- a/WEAT_results.xlsx
+++ b/WEAT_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saket/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D65CB6-D482-6242-B898-568F509EAED6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9927746F-41B1-A348-A714-ED2586E4746F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16600" activeTab="7" xr2:uid="{E4AD47C9-F031-C24A-9D0D-C939E375D1C2}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16600" activeTab="6" xr2:uid="{E4AD47C9-F031-C24A-9D0D-C939E375D1C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Career, Family" sheetId="1" r:id="rId1"/>
@@ -23,56 +23,35 @@
     <sheet name="Figure 5" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Figure 5'!$A$3:$B$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Figure 5'!$A$4:$B$4</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Figure 5'!$C$7:$H$7</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Figure 5'!$A$5:$B$5</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'Figure 5'!$A$3:$B$7</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'Figure 5'!$C$1:$C$2</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'Figure 5'!$C$3:$C$7</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'Figure 5'!$D$1:$D$2</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'Figure 5'!$D$3:$D$7</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Figure 5'!$A$6:$B$6</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'Figure 5'!$E$1:$E$2</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'Figure 5'!$E$3:$E$7</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'Figure 5'!$F$1:$F$2</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'Figure 5'!$F$3:$F$7</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'Figure 5'!$G$1:$G$2</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'Figure 5'!$G$3:$G$7</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'Figure 5'!$H$1:$H$2</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'Figure 5'!$H$3:$H$7</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Figure 5'!$A$7:$B$7</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Figure 5'!$C$1:$H$2</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Figure 5'!$C$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Figure 5'!$C$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Figure 5'!$C$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Figure 5'!$C$6:$H$6</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">'Figure 5'!$A$1:$B$7</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">'Figure 5'!$A$3:$B$7</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">'Figure 5'!$C$1:$C$2</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">'Figure 5'!$C$3:$C$7</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">'Figure 5'!$D$1:$D$2</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">'Figure 5'!$D$3:$D$7</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">'Figure 5'!$E$1:$E$2</definedName>
-    <definedName name="_xlchart.v2.18" hidden="1">'Figure 5'!$E$3:$E$7</definedName>
-    <definedName name="_xlchart.v2.19" hidden="1">'Figure 5'!$F$1:$F$2</definedName>
-    <definedName name="_xlchart.v2.20" hidden="1">'Figure 5'!$F$3:$F$7</definedName>
-    <definedName name="_xlchart.v2.21" hidden="1">'Figure 5'!$G$1:$G$2</definedName>
-    <definedName name="_xlchart.v2.22" hidden="1">'Figure 5'!$G$3:$G$7</definedName>
-    <definedName name="_xlchart.v2.23" hidden="1">'Figure 5'!$H$1:$H$2</definedName>
-    <definedName name="_xlchart.v2.24" hidden="1">'Figure 5'!$H$3:$H$7</definedName>
-    <definedName name="_xlchart.v2.38" hidden="1">'Figure 5'!$A$1:$H$2</definedName>
-    <definedName name="_xlchart.v2.39" hidden="1">'Figure 5'!$A$3:$B$3</definedName>
-    <definedName name="_xlchart.v2.40" hidden="1">'Figure 5'!$A$4:$B$4</definedName>
-    <definedName name="_xlchart.v2.41" hidden="1">'Figure 5'!$A$5:$B$5</definedName>
-    <definedName name="_xlchart.v2.42" hidden="1">'Figure 5'!$A$6:$B$6</definedName>
-    <definedName name="_xlchart.v2.43" hidden="1">'Figure 5'!$A$7:$B$7</definedName>
-    <definedName name="_xlchart.v2.44" hidden="1">'Figure 5'!$C$1:$H$2</definedName>
-    <definedName name="_xlchart.v2.45" hidden="1">'Figure 5'!$C$3:$H$3</definedName>
-    <definedName name="_xlchart.v2.46" hidden="1">'Figure 5'!$C$4:$H$4</definedName>
-    <definedName name="_xlchart.v2.47" hidden="1">'Figure 5'!$C$5:$H$5</definedName>
-    <definedName name="_xlchart.v2.48" hidden="1">'Figure 5'!$C$6:$H$6</definedName>
-    <definedName name="_xlchart.v2.49" hidden="1">'Figure 5'!$C$7:$H$7</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Figure 4'!$A$3:$B$7</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Figure 4'!$C$1:$C$2</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'Figure 4'!$A$3:$B$7</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'Figure 4'!$C$1:$C$2</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'Figure 4'!$C$3:$C$7</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'Figure 4'!$D$1:$D$2</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'Figure 4'!$D$3:$D$7</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Figure 4'!$C$3:$C$7</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'Figure 4'!$E$1:$E$2</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'Figure 4'!$E$3:$E$7</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'Figure 4'!$A$3:$B$7</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'Figure 4'!$C$1:$C$2</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'Figure 4'!$C$3:$C$7</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'Figure 4'!$D$1:$D$2</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'Figure 4'!$D$3:$D$7</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'Figure 4'!$E$1:$E$2</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'Figure 4'!$E$3:$E$7</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Figure 4'!$D$1:$D$2</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Figure 4'!$D$3:$D$7</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Figure 4'!$E$1:$E$2</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Figure 4'!$E$3:$E$7</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">'Figure 4'!$C$3:$C$7</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">'Figure 4'!$D$1:$D$2</definedName>
+    <definedName name="_xlchart.v2.12" hidden="1">'Figure 4'!$D$3:$D$7</definedName>
+    <definedName name="_xlchart.v2.13" hidden="1">'Figure 4'!$E$1:$E$2</definedName>
+    <definedName name="_xlchart.v2.14" hidden="1">'Figure 4'!$E$3:$E$7</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">'Figure 4'!$A$1:$B$7</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">'Figure 4'!$A$3:$B$7</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">'Figure 4'!$C$1:$C$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -89,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="24">
   <si>
     <t>Embedding</t>
   </si>
@@ -1753,8 +1732,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>ELMo - Gender Debiasing</a:t>
+              <a:t>ELMo</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Gender Debiasing</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1877,7 +1861,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A6FA-C848-BF2B-F2F39C516D1F}"/>
+              <c16:uniqueId val="{00000000-F69D-094C-94A5-C1BD88344289}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1890,10 +1874,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Without Debiasing</c:v>
+                  <c:v>Hard Debiasing</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>p</c:v>
+                  <c:v>d</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1945,16 +1929,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.7877000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.7878000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.7934000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.7902</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1964,7 +1948,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A6FA-C848-BF2B-F2F39C516D1F}"/>
+              <c16:uniqueId val="{00000001-F69D-094C-94A5-C1BD88344289}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1977,7 +1961,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Hard Debiasing</c:v>
+                  <c:v>Conceptor Debiasing</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>d</c:v>
@@ -2032,287 +2016,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.7877000000000001</c:v>
+                  <c:v>0.6966</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7878000000000001</c:v>
+                  <c:v>5.4899999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7934000000000001</c:v>
+                  <c:v>-0.60780000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7902</c:v>
+                  <c:v>-0.28050000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-0.84940000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A6FA-C848-BF2B-F2F39C516D1F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Figure 4'!$F$1:$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Hard Debiasing</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>p</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Figure 4'!$A$3:$B$7</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Pronouns</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Extended List</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Propernouns</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>All</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>AND</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Elmo</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Figure 4'!$F$3:$F$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-A6FA-C848-BF2B-F2F39C516D1F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Figure 4'!$G$1:$G$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Conceptor Debiasing</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>d</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Figure 4'!$A$3:$B$7</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Pronouns</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Extended List</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Propernouns</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>All</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>AND</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Elmo</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Figure 4'!$G$3:$G$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.6966</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.4899999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.60780000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.28050000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.84940000000000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-A6FA-C848-BF2B-F2F39C516D1F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Figure 4'!$H$1:$H$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Conceptor Debiasing</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>p</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Figure 4'!$A$3:$B$7</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Pronouns</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Extended List</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Propernouns</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>All</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>AND</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Elmo</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Figure 4'!$H$3:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9.8000000000000004E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.45700000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.88900000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.73</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.95499999999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-A6FA-C848-BF2B-F2F39C516D1F}"/>
+              <c16:uniqueId val="{00000002-F69D-094C-94A5-C1BD88344289}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2324,12 +2047,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="1628607984"/>
-        <c:axId val="1622403488"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1632280880"/>
+        <c:axId val="1634061184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1628607984"/>
+        <c:axId val="1632280880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2372,7 +2096,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1622403488"/>
+        <c:crossAx val="1634061184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2380,7 +2104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1622403488"/>
+        <c:axId val="1634061184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2431,7 +2155,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1628607984"/>
+        <c:crossAx val="1632280880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2444,7 +2168,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2546,8 +2270,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>BERT - Gender Debiasing</a:t>
+              <a:t>BERT - Gender</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Debiasing</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2670,7 +2399,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D664-9243-AA1E-2BE848CA8CCC}"/>
+              <c16:uniqueId val="{00000000-06F1-AE47-B485-D985F667E370}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2683,10 +2412,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Without Debiasing</c:v>
+                  <c:v>Hard Debiasing</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>p</c:v>
+                  <c:v>d</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2738,26 +2467,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>1.2067000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>1.2669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>1.2669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>1.2669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D664-9243-AA1E-2BE848CA8CCC}"/>
+              <c16:uniqueId val="{00000001-06F1-AE47-B485-D985F667E370}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2770,7 +2499,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Hard Debiasing</c:v>
+                  <c:v>Conceptor Debiasing</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>d</c:v>
@@ -2825,287 +2554,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.2067000000000001</c:v>
+                  <c:v>1.3108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2669999999999999</c:v>
+                  <c:v>1.3321000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2669999999999999</c:v>
+                  <c:v>0.91949999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2669999999999999</c:v>
+                  <c:v>0.62549999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.97270000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D664-9243-AA1E-2BE848CA8CCC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Figure 5'!$F$1:$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Hard Debiasing</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>p</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Figure 5'!$A$3:$B$7</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Pronouns</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Extended List</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Propernouns</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>All</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>AND</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Bert</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Figure 5'!$F$3:$F$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0000000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D664-9243-AA1E-2BE848CA8CCC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Figure 5'!$G$1:$G$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Conceptor Debiasing</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>d</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Figure 5'!$A$3:$B$7</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Pronouns</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Extended List</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Propernouns</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>All</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>AND</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Bert</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Figure 5'!$G$3:$G$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1.3108</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.3321000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.91949999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.62549999999999994</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.97270000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-D664-9243-AA1E-2BE848CA8CCC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Figure 5'!$H$1:$H$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Conceptor Debiasing</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>p</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Figure 5'!$A$3:$B$7</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Pronouns</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Extended List</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Propernouns</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>All</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>AND</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Bert</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Figure 5'!$H$3:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.6999999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.125</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7000000000000001E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D664-9243-AA1E-2BE848CA8CCC}"/>
+              <c16:uniqueId val="{00000002-06F1-AE47-B485-D985F667E370}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3117,12 +2585,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="1653161344"/>
-        <c:axId val="1630546464"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1653355552"/>
+        <c:axId val="1652978384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1653161344"/>
+        <c:axId val="1653355552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3165,7 +2634,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1630546464"/>
+        <c:crossAx val="1652978384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3173,7 +2642,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1630546464"/>
+        <c:axId val="1652978384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3224,7 +2693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1653161344"/>
+        <c:crossAx val="1653355552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3237,7 +2706,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5564,21 +5033,21 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E1BB97E-3764-CF49-BDBD-5F5706FB9B17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3CF4EB7-4ACD-0E4E-B60A-AE3715436B14}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5605,21 +5074,21 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CC5451B-5A97-D04B-9243-AD087CBD74E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3D3BF68-ACEE-2F41-8448-B15CF378CBE5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8850,57 +8319,45 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13404622-9A04-6249-BE48-7EE658CADAB2}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
@@ -8911,22 +8368,13 @@
         <v>1.7878000000000001</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>1.7877000000000001</v>
       </c>
       <c r="E3" s="4">
-        <v>1.7877000000000001</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
         <v>0.6966</v>
       </c>
-      <c r="H3" s="4">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -8935,22 +8383,13 @@
         <v>1.7878000000000001</v>
       </c>
       <c r="D4" s="4">
-        <v>0</v>
+        <v>1.7878000000000001</v>
       </c>
       <c r="E4" s="4">
-        <v>1.7878000000000001</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
         <v>5.4899999999999997E-2</v>
       </c>
-      <c r="H4" s="4">
-        <v>0.45700000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -8959,22 +8398,13 @@
         <v>1.7878000000000001</v>
       </c>
       <c r="D5" s="4">
-        <v>0</v>
+        <v>1.7934000000000001</v>
       </c>
       <c r="E5" s="4">
-        <v>1.7934000000000001</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
         <v>-0.60780000000000001</v>
       </c>
-      <c r="H5" s="4">
-        <v>0.88900000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -8983,22 +8413,13 @@
         <v>1.7878000000000001</v>
       </c>
       <c r="D6" s="4">
-        <v>0</v>
+        <v>1.7902</v>
       </c>
       <c r="E6" s="4">
-        <v>1.7902</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
         <v>-0.28050000000000003</v>
       </c>
-      <c r="H6" s="4">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
@@ -9006,30 +8427,18 @@
       <c r="C7" s="4">
         <v>1.7878000000000001</v>
       </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="E7" s="4">
         <v>-0.84940000000000004</v>
       </c>
-      <c r="H7" s="4">
-        <v>0.95499999999999996</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9038,57 +8447,45 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BBFD34-A36F-5F4C-A0BF-7C7191AE6667}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
@@ -9098,23 +8495,14 @@
       <c r="C3" s="4">
         <v>1.2068000000000001</v>
       </c>
-      <c r="D3" s="4">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="3">
         <v>1.2067000000000001</v>
       </c>
-      <c r="F3" s="3">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="E3" s="4">
         <v>1.3108</v>
       </c>
-      <c r="H3" s="4">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -9122,23 +8510,14 @@
       <c r="C4" s="4">
         <v>1.2068000000000001</v>
       </c>
-      <c r="D4" s="4">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="D4" s="3">
         <v>1.2669999999999999</v>
       </c>
-      <c r="F4" s="3">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="G4" s="4">
+      <c r="E4" s="4">
         <v>1.3321000000000001</v>
       </c>
-      <c r="H4" s="4">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -9146,23 +8525,14 @@
       <c r="C5" s="4">
         <v>1.2068000000000001</v>
       </c>
-      <c r="D5" s="4">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="3">
         <v>1.2669999999999999</v>
       </c>
-      <c r="F5" s="3">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="E5" s="4">
         <v>0.91949999999999998</v>
       </c>
-      <c r="H5" s="4">
-        <v>3.6999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -9170,23 +8540,14 @@
       <c r="C6" s="4">
         <v>1.2068000000000001</v>
       </c>
-      <c r="D6" s="4">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D6" s="3">
         <v>1.2669999999999999</v>
       </c>
-      <c r="F6" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="E6" s="4">
         <v>0.62549999999999994</v>
       </c>
-      <c r="H6" s="4">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
@@ -9194,30 +8555,18 @@
       <c r="C7" s="4">
         <v>1.2068000000000001</v>
       </c>
-      <c r="D7" s="4">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="E7" s="4">
         <v>0.97270000000000001</v>
       </c>
-      <c r="H7" s="4">
-        <v>1.7000000000000001E-2</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>